<commit_message>
# Modified Changed to Purchase Order Flow
Signed-off-by: ssrinivasan28 <sujitsrinivasan@outlook.com>
</commit_message>
<xml_diff>
--- a/IPMSWEB/test-input/PurchaseOrderManagement/Input_POEntry.xlsx
+++ b/IPMSWEB/test-input/PurchaseOrderManagement/Input_POEntry.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="6285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="12135"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" refMode="R1C1"/>
   <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t xml:space="preserve">Parameter </t>
   </si>
@@ -55,28 +55,19 @@
     <t>Vendor</t>
   </si>
   <si>
-    <t>055586</t>
-  </si>
-  <si>
     <t xml:space="preserve">SKU </t>
   </si>
   <si>
     <t xml:space="preserve">Purchase Qty </t>
   </si>
   <si>
-    <t>0000115675</t>
-  </si>
-  <si>
-    <t>SSR2109140</t>
+    <t>SSR032022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -138,14 +129,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +452,7 @@
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>700</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -476,7 +468,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -490,8 +482,8 @@
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
+      <c r="B4" s="4">
+        <v>586</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -515,34 +507,38 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="6">
+        <v>28787</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="6">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3">
-        <v>10</v>
-      </c>
-    </row>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>28787</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added PO Approval / PO Receving
Signed-off-by: ssrinivasan28 <sujitsrinivasan@outlook.com>
</commit_message>
<xml_diff>
--- a/IPMSWEB/test-input/PurchaseOrderManagement/Input_POEntry.xlsx
+++ b/IPMSWEB/test-input/PurchaseOrderManagement/Input_POEntry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="12135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11175" windowHeight="3525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Purchase Qty </t>
   </si>
   <si>
-    <t>SSR032022</t>
+    <t>SSR0302203</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +526,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="5">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>

</xml_diff>